<commit_message>
predicted per capita income and created csv file
</commit_message>
<xml_diff>
--- a/Linear-Regression/Excercise-Canada-per-capita-income/year.xlsx
+++ b/Linear-Regression/Excercise-Canada-per-capita-income/year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Hero Course Code\Machine-Learning\Linear-Regression\Excercise-Canada-per-capita-income\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3FB48F-642B-42FD-972B-866EFBB94AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA0EC0C-7A55-4280-877A-B5B956B9C5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,72 +345,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
         <v>2025</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
         <v>2026</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
         <v>2027</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
         <v>2028</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
         <v>2029</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
         <v>2030</v>
       </c>
     </row>

</xml_diff>